<commit_message>
Finished specification reader, started on operation generation.
</commit_message>
<xml_diff>
--- a/Specifications/Multiplication/22.xlsx
+++ b/Specifications/Multiplication/22.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderson1/Documents/personal projects/exercise sheets/Multiplication/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderson1/Google Drive/Documents/Coding/arithmetic-exercise-generator/specifications/multiplication/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21320" yWindow="460" windowWidth="27760" windowHeight="16380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="21420" yWindow="480" windowWidth="27760" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operand 1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -458,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>